<commit_message>
new graph/data for 10gbps, in rack, uneven, striping inception
</commit_message>
<xml_diff>
--- a/distributed-tensorflow-simulator/exp_results/inception-v3/graphs/10gbps_inrack_uneven_striping.xlsx
+++ b/distributed-tensorflow-simulator/exp_results/inception-v3/graphs/10gbps_inrack_uneven_striping.xlsx
@@ -62,16 +62,16 @@
     <t>0 Multicast</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1 Agg</t>
-  </si>
-  <si>
     <t>1 Multicast</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0 Agg</t>
+    <t>multicast + aggregation vs. multicast info</t>
   </si>
   <si>
-    <t>multicast + aggregation vs. multicast info</t>
+    <t>1 Agg</t>
+  </si>
+  <si>
+    <t>0 Agg</t>
   </si>
 </sst>
 </file>
@@ -258,19 +258,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.0779</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.9974</c:v>
+                    <c:v>3.2836</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.5519</c:v>
+                    <c:v>3.7941</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.8045</c:v>
+                    <c:v>3.8945</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.1873</c:v>
+                    <c:v>1.9033</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -282,19 +282,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.0912</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.407</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>3.9913</c:v>
+                    <c:v>8.4079</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>12.5747</c:v>
+                    <c:v>12.745</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>7.7287</c:v>
+                    <c:v>4.9452</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -347,16 +347,16 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2456</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.129</c:v>
+                  <c:v>17.5423</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28.4932</c:v>
+                  <c:v>27.7023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.9257</c:v>
+                  <c:v>35.6375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -414,10 +414,10 @@
                     <c:v>4.5732</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.1979</c:v>
+                    <c:v>2.9913</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.5571</c:v>
+                    <c:v>2.3382</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -438,10 +438,10 @@
                     <c:v>4.8032</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>26.6712</c:v>
+                    <c:v>0.8694</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.5363</c:v>
+                    <c:v>6.1606</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -500,10 +500,10 @@
                   <c:v>17.6742</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.9921</c:v>
+                  <c:v>30.6757</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.3253</c:v>
+                  <c:v>35.7977</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -552,19 +552,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>1.2781</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0205</c:v>
+                    <c:v>0.1508</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.585</c:v>
+                    <c:v>6.7194</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.2689</c:v>
+                    <c:v>3.5249</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.7446</c:v>
+                    <c:v>1.1707</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -576,19 +576,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.9627</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0204</c:v>
+                    <c:v>0.0133</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0</c:v>
+                    <c:v>0.0584</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.6042</c:v>
+                    <c:v>26.9899</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>11.919</c:v>
+                    <c:v>13.0162</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -638,19 +638,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>-0.4904</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>-0.0705</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0.0584</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.0519</c:v>
+                  <c:v>19.8606</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.8781</c:v>
+                  <c:v>33.0391</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -699,19 +699,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.4353</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0.6815</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0</c:v>
+                    <c:v>0.155</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>13.7889</c:v>
+                    <c:v>41.4111</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>15.2531</c:v>
+                    <c:v>4.1937</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -723,19 +723,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.3196</c:v>
+                    <c:v>0.2113</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0.9761</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0</c:v>
+                    <c:v>0.0283</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>9.5091</c:v>
+                    <c:v>9.3025</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>44.0996</c:v>
+                    <c:v>20.7719</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -785,19 +785,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>-0.0579</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0.1262</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.3866</c:v>
+                  <c:v>0.2458</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.4707</c:v>
+                  <c:v>17.3907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -812,11 +812,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2092259216"/>
-        <c:axId val="-2106561504"/>
+        <c:axId val="-2106070800"/>
+        <c:axId val="-2108586480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2092259216"/>
+        <c:axId val="-2106070800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -933,12 +933,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2106561504"/>
+        <c:crossAx val="-2108586480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2106561504"/>
+        <c:axId val="-2108586480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1068,7 +1068,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2092259216"/>
+        <c:crossAx val="-2106070800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1290,19 +1290,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.724</c:v>
+                    <c:v>0.4963</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.355</c:v>
+                    <c:v>0.1687</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.6026</c:v>
+                    <c:v>0.6782</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.525</c:v>
+                    <c:v>3.3384</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.5114</c:v>
+                    <c:v>1.3854</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1314,19 +1314,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.332</c:v>
+                    <c:v>1.0506</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.7429</c:v>
+                    <c:v>2.4275</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.4423</c:v>
+                    <c:v>0.5733</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.699</c:v>
+                    <c:v>1.8999</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.899</c:v>
+                    <c:v>1.2617</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1376,19 +1376,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>11.7545</c:v>
+                  <c:v>8.393</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9133</c:v>
+                  <c:v>21.5364</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.48</c:v>
+                  <c:v>32.3275</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39.5267</c:v>
+                  <c:v>41.9844</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.8443</c:v>
+                  <c:v>46.0874</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1437,19 +1437,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.6893</c:v>
+                    <c:v>0.0238</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1249</c:v>
+                    <c:v>0.2197</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.7713</c:v>
+                    <c:v>0.933</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.7809</c:v>
+                    <c:v>0.8437</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.5214</c:v>
+                    <c:v>1.1974</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1461,19 +1461,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.4916</c:v>
+                    <c:v>0.0486</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.5077</c:v>
+                    <c:v>3.0315</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.562</c:v>
+                    <c:v>0.6651</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.9686</c:v>
+                    <c:v>1.5857</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.4897</c:v>
+                    <c:v>0.7211</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1523,19 +1523,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>13.3262</c:v>
+                  <c:v>0.3331</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.0052</c:v>
+                  <c:v>26.1493</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.0271</c:v>
+                  <c:v>40.7364</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44.8913</c:v>
+                  <c:v>48.26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49.067</c:v>
+                  <c:v>51.291</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1584,19 +1584,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0849</c:v>
+                    <c:v>0.7904</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.237</c:v>
+                    <c:v>0.5128</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.599</c:v>
+                    <c:v>0.8812</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.6269</c:v>
+                    <c:v>8.535</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.4834</c:v>
+                    <c:v>0.8289</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1608,19 +1608,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1797</c:v>
+                    <c:v>0.5842</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.8322</c:v>
+                    <c:v>1.428</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.601</c:v>
+                    <c:v>0.9092</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.4193</c:v>
+                    <c:v>2.2585</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.7264</c:v>
+                    <c:v>0.8131</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1670,19 +1670,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.4333</c:v>
+                  <c:v>0.6597</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-14.8541</c:v>
+                  <c:v>11.7694</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.9014</c:v>
+                  <c:v>26.6038</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34.8332</c:v>
+                  <c:v>36.4248</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44.5055</c:v>
+                  <c:v>44.1225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1731,19 +1731,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.5778</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.12</c:v>
+                    <c:v>0.8622</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.8349</c:v>
+                    <c:v>0.7364</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>16.2451</c:v>
+                    <c:v>34.3139</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>13.4595</c:v>
+                    <c:v>0.842</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1755,19 +1755,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.0319</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.3298</c:v>
+                    <c:v>0.5418</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.8904</c:v>
+                    <c:v>0.682</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>54.3345</c:v>
+                    <c:v>19.5926</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>24.0024</c:v>
+                    <c:v>9.5029</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1817,19 +1817,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>-0.0792</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.545</c:v>
+                  <c:v>0.9222</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-10.9501</c:v>
+                  <c:v>10.9688</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.3943</c:v>
+                  <c:v>27.0264</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.4</c:v>
+                  <c:v>37.5762</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1844,11 +1844,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2072871872"/>
-        <c:axId val="-2093553152"/>
+        <c:axId val="-2103936240"/>
+        <c:axId val="-2103929984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2072871872"/>
+        <c:axId val="-2103936240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1965,12 +1965,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093553152"/>
+        <c:crossAx val="-2103929984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093553152"/>
+        <c:axId val="-2103929984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2100,7 +2100,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2072871872"/>
+        <c:crossAx val="-2103936240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2322,19 +2322,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.724</c:v>
+                    <c:v>0.4963</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.7574</c:v>
+                    <c:v>3.4201</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.3294</c:v>
+                    <c:v>4.3108</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.3667</c:v>
+                    <c:v>1.5144</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.7237</c:v>
+                    <c:v>0.9357</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2346,19 +2346,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.332</c:v>
+                    <c:v>1.0506</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.0678</c:v>
+                    <c:v>2.4597</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.663299999999999</c:v>
+                    <c:v>4.6616</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>17.129</c:v>
+                    <c:v>6.5517</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.3712</c:v>
+                    <c:v>3.7612</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2408,19 +2408,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>11.7545</c:v>
+                  <c:v>8.393</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0258</c:v>
+                  <c:v>21.5686</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48.6616</c:v>
+                  <c:v>51.595</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>72.9019</c:v>
+                  <c:v>74.0996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>86.0782</c:v>
+                  <c:v>86.1111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2469,19 +2469,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.6893</c:v>
+                    <c:v>0.0238</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.4495</c:v>
+                    <c:v>3.5396</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>3.9687</c:v>
+                    <c:v>3.8494</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.932</c:v>
+                    <c:v>0.1876</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.0587</c:v>
+                    <c:v>0.1219</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2493,19 +2493,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.4916</c:v>
+                    <c:v>0.0486</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.5278</c:v>
+                    <c:v>3.0719</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.2807</c:v>
+                    <c:v>4.1776</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>5.0841</c:v>
+                    <c:v>0.4435</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>13.6145</c:v>
+                    <c:v>13.6037</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2555,19 +2555,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>13.3262</c:v>
+                  <c:v>0.3331</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.0253</c:v>
+                  <c:v>26.1897</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51.9501</c:v>
+                  <c:v>58.7179</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75.4802</c:v>
+                  <c:v>77.9715</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>87.1549</c:v>
+                  <c:v>88.8758</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2616,19 +2616,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0849</c:v>
+                    <c:v>0.7904</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.237</c:v>
+                    <c:v>0.5128</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.2328</c:v>
+                    <c:v>6.2503</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.8308</c:v>
+                    <c:v>5.9524</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.4266</c:v>
+                    <c:v>0.654</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2640,19 +2640,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1797</c:v>
+                    <c:v>0.5842</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.8322</c:v>
+                    <c:v>1.428</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.9532</c:v>
+                    <c:v>1.4247</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6.726</c:v>
+                    <c:v>26.1351</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.6759</c:v>
+                    <c:v>8.83</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2702,19 +2702,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.4333</c:v>
+                  <c:v>0.6597</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-14.8541</c:v>
+                  <c:v>11.7694</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.2536</c:v>
+                  <c:v>27.1193</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54.5555</c:v>
+                  <c:v>54.1593</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>77.2114</c:v>
+                  <c:v>77.5492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2763,19 +2763,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.5778</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.12</c:v>
+                    <c:v>0.8622</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.8349</c:v>
+                    <c:v>0.7364</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>10.3684</c:v>
+                    <c:v>30.5061</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>8.9168</c:v>
+                    <c:v>0.4658</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2787,19 +2787,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.0319</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.3298</c:v>
+                    <c:v>0.5418</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.8904</c:v>
+                    <c:v>0.682</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.1291</c:v>
+                    <c:v>12.2631</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>13.6537</c:v>
+                    <c:v>4.2102</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2849,19 +2849,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>-0.0792</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.545</c:v>
+                  <c:v>0.9222</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-10.9501</c:v>
+                  <c:v>10.9688</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.4546</c:v>
+                  <c:v>28.2392</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>56.5838</c:v>
+                  <c:v>57.9314</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2876,11 +2876,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2050318192"/>
-        <c:axId val="-2051400144"/>
+        <c:axId val="-2103871344"/>
+        <c:axId val="-2103865088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2050318192"/>
+        <c:axId val="-2103871344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2997,12 +2997,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2051400144"/>
+        <c:crossAx val="-2103865088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2051400144"/>
+        <c:axId val="-2103865088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3132,7 +3132,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2050318192"/>
+        <c:crossAx val="-2103871344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3354,19 +3354,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.0202</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.9343</c:v>
+                    <c:v>4.1939</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.6866</c:v>
+                    <c:v>6.9352</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.4339</c:v>
+                    <c:v>0.6827</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.4348</c:v>
+                    <c:v>1.94</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3384,13 +3384,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.1654</c:v>
+                    <c:v>7.465</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>28.687</c:v>
+                    <c:v>8.9237</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>9.0913</c:v>
+                    <c:v>6.4278</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3446,13 +3446,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.0684</c:v>
+                  <c:v>28.2545</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55.047</c:v>
+                  <c:v>54.7173</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>74.048</c:v>
+                  <c:v>74.0337</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3504,16 +3504,16 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.8503</c:v>
+                    <c:v>4.5637</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.6586</c:v>
+                    <c:v>7.3087</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.9112</c:v>
+                    <c:v>1.5184</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.6498</c:v>
+                    <c:v>0.4937</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3531,13 +3531,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.1423</c:v>
+                    <c:v>7.9035</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>8.9312</c:v>
+                    <c:v>0.6049</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>26.2655</c:v>
+                    <c:v>28.0233</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3593,13 +3593,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.8826</c:v>
+                  <c:v>29.969</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56.1299</c:v>
+                  <c:v>57.1723</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>74.4155</c:v>
+                  <c:v>77.1619</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3654,13 +3654,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>9.0192</c:v>
+                    <c:v>9.2181</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.9538</c:v>
+                    <c:v>6.1464</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.3427</c:v>
+                    <c:v>0.9307</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3681,10 +3681,10 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.4959</c:v>
+                    <c:v>38.0281</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.994</c:v>
+                    <c:v>15.0583</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3743,10 +3743,10 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.8572</c:v>
+                  <c:v>27.5288</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>58.7004</c:v>
+                  <c:v>59.8579</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3804,10 +3804,10 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>38.8934</c:v>
+                    <c:v>15.1643</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>11.7645</c:v>
+                    <c:v>8.8231</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3828,10 +3828,10 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>8.5667</c:v>
+                    <c:v>21.3811</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>21.7742</c:v>
+                    <c:v>3.7778</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3890,10 +3890,10 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.824</c:v>
+                  <c:v>-0.3175</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31.769</c:v>
+                  <c:v>32.608</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3908,11 +3908,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2095164416"/>
-        <c:axId val="-2026839152"/>
+        <c:axId val="-2103806640"/>
+        <c:axId val="-2103800384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2095164416"/>
+        <c:axId val="-2103806640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4029,12 +4029,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2026839152"/>
+        <c:crossAx val="-2103800384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2026839152"/>
+        <c:axId val="-2103800384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4164,7 +4164,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2095164416"/>
+        <c:crossAx val="-2103806640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6871,8 +6871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6919,7 +6919,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -6939,10 +6939,10 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>1.0911999999999999</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>1.0779000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -6959,13 +6959,13 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>1.2456</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>1.407</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0.99739999999999995</v>
+        <v>3.2835999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -6982,13 +6982,13 @@
         <v>8</v>
       </c>
       <c r="E6">
-        <v>16.129000000000001</v>
+        <v>17.542300000000001</v>
       </c>
       <c r="F6">
-        <v>3.9912999999999998</v>
+        <v>8.4078999999999997</v>
       </c>
       <c r="G6">
-        <v>4.5518999999999998</v>
+        <v>3.7940999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -7005,13 +7005,13 @@
         <v>16</v>
       </c>
       <c r="E7">
-        <v>28.493200000000002</v>
+        <v>27.702300000000001</v>
       </c>
       <c r="F7">
-        <v>12.5747</v>
+        <v>12.744999999999999</v>
       </c>
       <c r="G7">
-        <v>2.8045</v>
+        <v>3.8944999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -7028,13 +7028,13 @@
         <v>32</v>
       </c>
       <c r="E8">
-        <v>36.925699999999999</v>
+        <v>35.637500000000003</v>
       </c>
       <c r="F8">
-        <v>7.7286999999999999</v>
+        <v>4.9451999999999998</v>
       </c>
       <c r="G8">
-        <v>1.1873</v>
+        <v>1.9033</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -7120,13 +7120,13 @@
         <v>16</v>
       </c>
       <c r="E13">
-        <v>29.992100000000001</v>
+        <v>30.675699999999999</v>
       </c>
       <c r="F13">
-        <v>26.671199999999999</v>
+        <v>0.86939999999999995</v>
       </c>
       <c r="G13">
-        <v>2.1979000000000002</v>
+        <v>2.9912999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -7143,13 +7143,13 @@
         <v>32</v>
       </c>
       <c r="E14">
-        <v>37.325299999999999</v>
+        <v>35.797699999999999</v>
       </c>
       <c r="F14">
-        <v>3.5363000000000002</v>
+        <v>6.1605999999999996</v>
       </c>
       <c r="G14">
-        <v>0.55710000000000004</v>
+        <v>2.3382000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -7166,13 +7166,13 @@
         <v>2</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>-0.4904</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>0.9627</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>1.2781</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -7189,13 +7189,13 @@
         <v>4</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>-7.0499999999999993E-2</v>
       </c>
       <c r="F17">
-        <v>2.0400000000000001E-2</v>
+        <v>1.3299999999999999E-2</v>
       </c>
       <c r="G17">
-        <v>2.0500000000000001E-2</v>
+        <v>0.15079999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -7212,13 +7212,13 @@
         <v>8</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>5.8400000000000001E-2</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>5.8400000000000001E-2</v>
       </c>
       <c r="G18">
-        <v>7.585</v>
+        <v>6.7194000000000003</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -7235,13 +7235,13 @@
         <v>16</v>
       </c>
       <c r="E19">
-        <v>18.0519</v>
+        <v>19.860600000000002</v>
       </c>
       <c r="F19">
-        <v>1.6042000000000001</v>
+        <v>26.989899999999999</v>
       </c>
       <c r="G19">
-        <v>3.2688999999999999</v>
+        <v>3.5249000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -7258,13 +7258,13 @@
         <v>32</v>
       </c>
       <c r="E20">
-        <v>32.878100000000003</v>
+        <v>33.039099999999998</v>
       </c>
       <c r="F20">
-        <v>11.919</v>
+        <v>13.0162</v>
       </c>
       <c r="G20">
-        <v>2.7446000000000002</v>
+        <v>1.1707000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -7281,13 +7281,13 @@
         <v>2</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>-5.79E-2</v>
       </c>
       <c r="F22">
-        <v>0.3196</v>
+        <v>0.21129999999999999</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>0.43530000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -7304,13 +7304,13 @@
         <v>4</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>0.12620000000000001</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>0.97609999999999997</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>0.68149999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -7330,10 +7330,10 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>2.8299999999999999E-2</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>0.155</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -7350,13 +7350,13 @@
         <v>16</v>
       </c>
       <c r="E25">
-        <v>-1.3866000000000001</v>
+        <v>0.24579999999999999</v>
       </c>
       <c r="F25">
-        <v>9.5091000000000001</v>
+        <v>9.3025000000000002</v>
       </c>
       <c r="G25">
-        <v>13.7889</v>
+        <v>41.411099999999998</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -7373,21 +7373,21 @@
         <v>32</v>
       </c>
       <c r="E26">
-        <v>20.470700000000001</v>
+        <v>17.390699999999999</v>
       </c>
       <c r="F26">
-        <v>44.099600000000002</v>
+        <v>20.771899999999999</v>
       </c>
       <c r="G26">
-        <v>15.2531</v>
+        <v>4.1936999999999998</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -7404,13 +7404,13 @@
         <v>2</v>
       </c>
       <c r="E29">
-        <v>11.7545</v>
+        <v>8.3930000000000007</v>
       </c>
       <c r="F29">
-        <v>1.3320000000000001</v>
+        <v>1.0506</v>
       </c>
       <c r="G29">
-        <v>1.724</v>
+        <v>0.49630000000000002</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -7427,13 +7427,13 @@
         <v>4</v>
       </c>
       <c r="E30">
-        <v>9.9132999999999996</v>
+        <v>21.5364</v>
       </c>
       <c r="F30">
-        <v>1.7428999999999999</v>
+        <v>2.4275000000000002</v>
       </c>
       <c r="G30">
-        <v>1.355</v>
+        <v>0.16869999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -7450,13 +7450,13 @@
         <v>8</v>
       </c>
       <c r="E31">
-        <v>29.48</v>
+        <v>32.327500000000001</v>
       </c>
       <c r="F31">
-        <v>0.44230000000000003</v>
+        <v>0.57330000000000003</v>
       </c>
       <c r="G31">
-        <v>0.60260000000000002</v>
+        <v>0.67820000000000003</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -7473,13 +7473,13 @@
         <v>16</v>
       </c>
       <c r="E32">
-        <v>39.526699999999998</v>
+        <v>41.984400000000001</v>
       </c>
       <c r="F32">
-        <v>0.69899999999999995</v>
+        <v>1.8998999999999999</v>
       </c>
       <c r="G32">
-        <v>1.5249999999999999</v>
+        <v>3.3384</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -7496,13 +7496,13 @@
         <v>32</v>
       </c>
       <c r="E33">
-        <v>45.844299999999997</v>
+        <v>46.087400000000002</v>
       </c>
       <c r="F33">
-        <v>0.89900000000000002</v>
+        <v>1.2617</v>
       </c>
       <c r="G33">
-        <v>0.51139999999999997</v>
+        <v>1.3854</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -7519,13 +7519,13 @@
         <v>2</v>
       </c>
       <c r="E35">
-        <v>13.3262</v>
+        <v>0.33310000000000001</v>
       </c>
       <c r="F35">
-        <v>1.4916</v>
+        <v>4.8599999999999997E-2</v>
       </c>
       <c r="G35">
-        <v>0.68930000000000002</v>
+        <v>2.3800000000000002E-2</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -7542,13 +7542,13 @@
         <v>4</v>
       </c>
       <c r="E36">
-        <v>13.0052</v>
+        <v>26.1493</v>
       </c>
       <c r="F36">
-        <v>1.5077</v>
+        <v>3.0314999999999999</v>
       </c>
       <c r="G36">
-        <v>0.1249</v>
+        <v>0.21970000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -7565,13 +7565,13 @@
         <v>8</v>
       </c>
       <c r="E37">
-        <v>34.027099999999997</v>
+        <v>40.736400000000003</v>
       </c>
       <c r="F37">
-        <v>0.56200000000000006</v>
+        <v>0.66510000000000002</v>
       </c>
       <c r="G37">
-        <v>0.77129999999999999</v>
+        <v>0.93300000000000005</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -7588,13 +7588,13 @@
         <v>16</v>
       </c>
       <c r="E38">
-        <v>44.891300000000001</v>
+        <v>48.26</v>
       </c>
       <c r="F38">
-        <v>1.9685999999999999</v>
+        <v>1.5857000000000001</v>
       </c>
       <c r="G38">
-        <v>0.78090000000000004</v>
+        <v>0.84370000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -7611,13 +7611,13 @@
         <v>32</v>
       </c>
       <c r="E39">
-        <v>49.067</v>
+        <v>51.290999999999997</v>
       </c>
       <c r="F39">
-        <v>0.48970000000000002</v>
+        <v>0.72109999999999996</v>
       </c>
       <c r="G39">
-        <v>1.5214000000000001</v>
+        <v>1.1974</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -7634,13 +7634,13 @@
         <v>2</v>
       </c>
       <c r="E41">
-        <v>1.4333</v>
+        <v>0.65969999999999995</v>
       </c>
       <c r="F41">
-        <v>0.1797</v>
+        <v>0.58420000000000005</v>
       </c>
       <c r="G41">
-        <v>8.4900000000000003E-2</v>
+        <v>0.79039999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -7657,13 +7657,13 @@
         <v>4</v>
       </c>
       <c r="E42">
-        <v>-14.854100000000001</v>
+        <v>11.769399999999999</v>
       </c>
       <c r="F42">
-        <v>0.83220000000000005</v>
+        <v>1.4279999999999999</v>
       </c>
       <c r="G42">
-        <v>2.2370000000000001</v>
+        <v>0.51280000000000003</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -7680,13 +7680,13 @@
         <v>8</v>
       </c>
       <c r="E43">
-        <v>15.901400000000001</v>
+        <v>26.6038</v>
       </c>
       <c r="F43">
-        <v>0.60099999999999998</v>
+        <v>0.90920000000000001</v>
       </c>
       <c r="G43">
-        <v>0.59899999999999998</v>
+        <v>0.88119999999999998</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -7703,13 +7703,13 @@
         <v>16</v>
       </c>
       <c r="E44">
-        <v>34.833199999999998</v>
+        <v>36.424799999999998</v>
       </c>
       <c r="F44">
-        <v>3.4192999999999998</v>
+        <v>2.2585000000000002</v>
       </c>
       <c r="G44">
-        <v>0.62690000000000001</v>
+        <v>8.5350000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -7726,13 +7726,13 @@
         <v>32</v>
       </c>
       <c r="E45">
-        <v>44.505499999999998</v>
+        <v>44.122500000000002</v>
       </c>
       <c r="F45">
-        <v>0.72640000000000005</v>
+        <v>0.81310000000000004</v>
       </c>
       <c r="G45">
-        <v>0.4834</v>
+        <v>0.82889999999999997</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -7749,13 +7749,13 @@
         <v>2</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>-7.9200000000000007E-2</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>3.1899999999999998E-2</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>0.57779999999999998</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -7772,13 +7772,13 @@
         <v>4</v>
       </c>
       <c r="E48">
-        <v>2.5449999999999999</v>
+        <v>0.92220000000000002</v>
       </c>
       <c r="F48">
-        <v>0.32979999999999998</v>
+        <v>0.54179999999999995</v>
       </c>
       <c r="G48">
-        <v>0.12</v>
+        <v>0.86219999999999997</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -7795,13 +7795,13 @@
         <v>8</v>
       </c>
       <c r="E49">
-        <v>-10.950100000000001</v>
+        <v>10.9688</v>
       </c>
       <c r="F49">
-        <v>0.89039999999999997</v>
+        <v>0.68200000000000005</v>
       </c>
       <c r="G49">
-        <v>0.83489999999999998</v>
+        <v>0.73640000000000005</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -7818,13 +7818,13 @@
         <v>16</v>
       </c>
       <c r="E50">
-        <v>16.394300000000001</v>
+        <v>27.026399999999999</v>
       </c>
       <c r="F50">
-        <v>54.334499999999998</v>
+        <v>19.592600000000001</v>
       </c>
       <c r="G50">
-        <v>16.245100000000001</v>
+        <v>34.313899999999997</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -7841,21 +7841,21 @@
         <v>32</v>
       </c>
       <c r="E51">
-        <v>36.4</v>
+        <v>37.5762</v>
       </c>
       <c r="F51">
-        <v>24.002400000000002</v>
+        <v>9.5029000000000003</v>
       </c>
       <c r="G51">
-        <v>13.4595</v>
+        <v>0.84199999999999997</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B53" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -7872,13 +7872,13 @@
         <v>2</v>
       </c>
       <c r="E54">
-        <v>11.7545</v>
+        <v>8.3930000000000007</v>
       </c>
       <c r="F54">
-        <v>1.3320000000000001</v>
+        <v>1.0506</v>
       </c>
       <c r="G54">
-        <v>1.724</v>
+        <v>0.49630000000000002</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -7895,13 +7895,13 @@
         <v>4</v>
       </c>
       <c r="E55">
-        <v>10.0258</v>
+        <v>21.5686</v>
       </c>
       <c r="F55">
-        <v>1.0678000000000001</v>
+        <v>2.4597000000000002</v>
       </c>
       <c r="G55">
-        <v>1.7574000000000001</v>
+        <v>3.4201000000000001</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -7918,13 +7918,13 @@
         <v>8</v>
       </c>
       <c r="E56">
-        <v>48.6616</v>
+        <v>51.594999999999999</v>
       </c>
       <c r="F56">
-        <v>4.6632999999999996</v>
+        <v>4.6616</v>
       </c>
       <c r="G56">
-        <v>4.3293999999999997</v>
+        <v>4.3108000000000004</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -7941,13 +7941,13 @@
         <v>16</v>
       </c>
       <c r="E57">
-        <v>72.901899999999998</v>
+        <v>74.099599999999995</v>
       </c>
       <c r="F57">
-        <v>17.129000000000001</v>
+        <v>6.5517000000000003</v>
       </c>
       <c r="G57">
-        <v>2.3666999999999998</v>
+        <v>1.5144</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -7964,13 +7964,13 @@
         <v>32</v>
       </c>
       <c r="E58">
-        <v>86.078199999999995</v>
+        <v>86.111099999999993</v>
       </c>
       <c r="F58">
-        <v>5.3712</v>
+        <v>3.7612000000000001</v>
       </c>
       <c r="G58">
-        <v>1.7237</v>
+        <v>0.93569999999999998</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -7987,13 +7987,13 @@
         <v>2</v>
       </c>
       <c r="E60">
-        <v>13.3262</v>
+        <v>0.33310000000000001</v>
       </c>
       <c r="F60">
-        <v>1.4916</v>
+        <v>4.8599999999999997E-2</v>
       </c>
       <c r="G60">
-        <v>0.68930000000000002</v>
+        <v>2.3800000000000002E-2</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -8010,13 +8010,13 @@
         <v>4</v>
       </c>
       <c r="E61">
-        <v>13.0253</v>
+        <v>26.189699999999998</v>
       </c>
       <c r="F61">
-        <v>1.5278</v>
+        <v>3.0718999999999999</v>
       </c>
       <c r="G61">
-        <v>3.4495</v>
+        <v>3.5396000000000001</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -8033,13 +8033,13 @@
         <v>8</v>
       </c>
       <c r="E62">
-        <v>51.950099999999999</v>
+        <v>58.7179</v>
       </c>
       <c r="F62">
-        <v>4.2807000000000004</v>
+        <v>4.1776</v>
       </c>
       <c r="G62">
-        <v>3.9687000000000001</v>
+        <v>3.8494000000000002</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -8056,13 +8056,13 @@
         <v>16</v>
       </c>
       <c r="E63">
-        <v>75.480199999999996</v>
+        <v>77.971500000000006</v>
       </c>
       <c r="F63">
-        <v>5.0841000000000003</v>
+        <v>0.44350000000000001</v>
       </c>
       <c r="G63">
-        <v>0.93200000000000005</v>
+        <v>0.18759999999999999</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -8079,13 +8079,13 @@
         <v>32</v>
       </c>
       <c r="E64">
-        <v>87.154899999999998</v>
+        <v>88.875799999999998</v>
       </c>
       <c r="F64">
-        <v>13.6145</v>
+        <v>13.6037</v>
       </c>
       <c r="G64">
-        <v>5.8700000000000002E-2</v>
+        <v>0.12189999999999999</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -8102,13 +8102,13 @@
         <v>2</v>
       </c>
       <c r="E66">
-        <v>1.4333</v>
+        <v>0.65969999999999995</v>
       </c>
       <c r="F66">
-        <v>0.1797</v>
+        <v>0.58420000000000005</v>
       </c>
       <c r="G66">
-        <v>8.4900000000000003E-2</v>
+        <v>0.79039999999999999</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -8125,13 +8125,13 @@
         <v>4</v>
       </c>
       <c r="E67">
-        <v>-14.854100000000001</v>
+        <v>11.769399999999999</v>
       </c>
       <c r="F67">
-        <v>0.83220000000000005</v>
+        <v>1.4279999999999999</v>
       </c>
       <c r="G67">
-        <v>2.2370000000000001</v>
+        <v>0.51280000000000003</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -8148,13 +8148,13 @@
         <v>8</v>
       </c>
       <c r="E68">
-        <v>16.253599999999999</v>
+        <v>27.119299999999999</v>
       </c>
       <c r="F68">
-        <v>0.95320000000000005</v>
+        <v>1.4247000000000001</v>
       </c>
       <c r="G68">
-        <v>7.2328000000000001</v>
+        <v>6.2503000000000002</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -8171,13 +8171,13 @@
         <v>16</v>
       </c>
       <c r="E69">
-        <v>54.555500000000002</v>
+        <v>54.159300000000002</v>
       </c>
       <c r="F69">
-        <v>6.726</v>
+        <v>26.135100000000001</v>
       </c>
       <c r="G69">
-        <v>3.8308</v>
+        <v>5.9523999999999999</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -8194,13 +8194,13 @@
         <v>32</v>
       </c>
       <c r="E70">
-        <v>77.211399999999998</v>
+        <v>77.549199999999999</v>
       </c>
       <c r="F70">
-        <v>2.6758999999999999</v>
+        <v>8.83</v>
       </c>
       <c r="G70">
-        <v>0.42659999999999998</v>
+        <v>0.65400000000000003</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -8217,13 +8217,13 @@
         <v>2</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>-7.9200000000000007E-2</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>3.1899999999999998E-2</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>0.57779999999999998</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -8240,13 +8240,13 @@
         <v>4</v>
       </c>
       <c r="E73">
-        <v>2.5449999999999999</v>
+        <v>0.92220000000000002</v>
       </c>
       <c r="F73">
-        <v>0.32979999999999998</v>
+        <v>0.54179999999999995</v>
       </c>
       <c r="G73">
-        <v>0.12</v>
+        <v>0.86219999999999997</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -8263,13 +8263,13 @@
         <v>8</v>
       </c>
       <c r="E74">
-        <v>-10.950100000000001</v>
+        <v>10.9688</v>
       </c>
       <c r="F74">
-        <v>0.89039999999999997</v>
+        <v>0.68200000000000005</v>
       </c>
       <c r="G74">
-        <v>0.83489999999999998</v>
+        <v>0.73640000000000005</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -8286,13 +8286,13 @@
         <v>16</v>
       </c>
       <c r="E75">
-        <v>18.454599999999999</v>
+        <v>28.2392</v>
       </c>
       <c r="F75">
-        <v>4.1291000000000002</v>
+        <v>12.2631</v>
       </c>
       <c r="G75">
-        <v>10.368399999999999</v>
+        <v>30.5061</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -8309,18 +8309,18 @@
         <v>32</v>
       </c>
       <c r="E76">
-        <v>56.583799999999997</v>
+        <v>57.931399999999996</v>
       </c>
       <c r="F76">
-        <v>13.653700000000001</v>
+        <v>4.2102000000000004</v>
       </c>
       <c r="G76">
-        <v>8.9168000000000003</v>
+        <v>0.46579999999999999</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
@@ -8343,7 +8343,7 @@
         <v>0</v>
       </c>
       <c r="G79">
-        <v>0</v>
+        <v>2.0199999999999999E-2</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -8366,7 +8366,7 @@
         <v>0</v>
       </c>
       <c r="G80">
-        <v>3.9342999999999999</v>
+        <v>4.1939000000000002</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -8383,13 +8383,13 @@
         <v>8</v>
       </c>
       <c r="E81">
-        <v>27.0684</v>
+        <v>28.2545</v>
       </c>
       <c r="F81">
-        <v>7.1654</v>
+        <v>7.4649999999999999</v>
       </c>
       <c r="G81">
-        <v>6.6866000000000003</v>
+        <v>6.9352</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -8406,13 +8406,13 @@
         <v>16</v>
       </c>
       <c r="E82">
-        <v>55.046999999999997</v>
+        <v>54.717300000000002</v>
       </c>
       <c r="F82">
-        <v>28.687000000000001</v>
+        <v>8.9237000000000002</v>
       </c>
       <c r="G82">
-        <v>4.4339000000000004</v>
+        <v>0.68269999999999997</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -8429,13 +8429,13 @@
         <v>32</v>
       </c>
       <c r="E83">
-        <v>74.048000000000002</v>
+        <v>74.033699999999996</v>
       </c>
       <c r="F83">
-        <v>9.0913000000000004</v>
+        <v>6.4278000000000004</v>
       </c>
       <c r="G83">
-        <v>3.4348000000000001</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -8481,7 +8481,7 @@
         <v>0</v>
       </c>
       <c r="G86">
-        <v>3.8502999999999998</v>
+        <v>4.5636999999999999</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
@@ -8498,13 +8498,13 @@
         <v>8</v>
       </c>
       <c r="E87">
-        <v>26.8826</v>
+        <v>29.969000000000001</v>
       </c>
       <c r="F87">
-        <v>7.1422999999999996</v>
+        <v>7.9035000000000002</v>
       </c>
       <c r="G87">
-        <v>6.6585999999999999</v>
+        <v>7.3087</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -8521,13 +8521,13 @@
         <v>16</v>
       </c>
       <c r="E88">
-        <v>56.129899999999999</v>
+        <v>57.1723</v>
       </c>
       <c r="F88">
-        <v>8.9312000000000005</v>
+        <v>0.60489999999999999</v>
       </c>
       <c r="G88">
-        <v>0.91120000000000001</v>
+        <v>1.5184</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -8544,13 +8544,13 @@
         <v>32</v>
       </c>
       <c r="E89">
-        <v>74.415499999999994</v>
+        <v>77.161900000000003</v>
       </c>
       <c r="F89">
-        <v>26.265499999999999</v>
+        <v>28.023299999999999</v>
       </c>
       <c r="G89">
-        <v>0.64980000000000004</v>
+        <v>0.49370000000000003</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -8619,7 +8619,7 @@
         <v>0</v>
       </c>
       <c r="G93">
-        <v>9.0191999999999997</v>
+        <v>9.2180999999999997</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -8636,13 +8636,13 @@
         <v>16</v>
       </c>
       <c r="E94">
-        <v>30.857199999999999</v>
+        <v>27.5288</v>
       </c>
       <c r="F94">
-        <v>7.4958999999999998</v>
+        <v>38.028100000000002</v>
       </c>
       <c r="G94">
-        <v>4.9538000000000002</v>
+        <v>6.1463999999999999</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -8659,13 +8659,13 @@
         <v>32</v>
       </c>
       <c r="E95">
-        <v>58.700400000000002</v>
+        <v>59.857900000000001</v>
       </c>
       <c r="F95">
-        <v>3.9940000000000002</v>
+        <v>15.058299999999999</v>
       </c>
       <c r="G95">
-        <v>1.3427</v>
+        <v>0.93069999999999997</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -8751,13 +8751,13 @@
         <v>16</v>
       </c>
       <c r="E100">
-        <v>1.8240000000000001</v>
+        <v>-0.3175</v>
       </c>
       <c r="F100">
-        <v>8.5667000000000009</v>
+        <v>21.3811</v>
       </c>
       <c r="G100">
-        <v>38.8934</v>
+        <v>15.164300000000001</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -8774,13 +8774,13 @@
         <v>32</v>
       </c>
       <c r="E101">
-        <v>31.768999999999998</v>
+        <v>32.607999999999997</v>
       </c>
       <c r="F101">
-        <v>21.7742</v>
+        <v>3.7778</v>
       </c>
       <c r="G101">
-        <v>11.7645</v>
+        <v>8.8231000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated graph styles for inception 10gbps, in rack, uneven, striping
</commit_message>
<xml_diff>
--- a/distributed-tensorflow-simulator/exp_results/inception-v3/graphs/10gbps_inrack_uneven_striping.xlsx
+++ b/distributed-tensorflow-simulator/exp_results/inception-v3/graphs/10gbps_inrack_uneven_striping.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>multicast</t>
   </si>
@@ -73,17 +73,41 @@
   <si>
     <t>0 Agg</t>
   </si>
+  <si>
+    <t>Inception-V3: Aggregation/No Multicast vs Baseline</t>
+  </si>
+  <si>
+    <t>Inception-V3: Multicast/No Aggregation vs Baseline)</t>
+  </si>
+  <si>
+    <t>Inception-V3: Aggregation/Multicast vs Baseline</t>
+  </si>
+  <si>
+    <t>Inception-V3: Multicast+Agg vs Multicast</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -107,8 +131,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -137,82 +167,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Inception-V3: Percentage</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t> Improvement vs. Number of Workers (Aggregation/No Multicast vs Baseline)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1600" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.102694892196067"/>
+          <c:y val="0.0274856997713995"/>
+          <c:w val="0.866779211499086"/>
+          <c:h val="0.847606807213614"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -223,7 +190,7 @@
             <c:v>1 PS</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="41275" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -235,84 +202,13 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>out!$G$4:$G$8</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>3.2836</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>3.7941</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3.8945</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>1.9033</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>out!$F$4:$F$8</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>8.4079</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>12.745</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>4.9452</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>out!$D$4:$D$8</c:f>
@@ -370,10 +266,11 @@
             <c:v>2 PS</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="41275" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="C00000"/>
               </a:solidFill>
+              <a:prstDash val="lgDashDotDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -382,84 +279,13 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>out!$G$10:$G$14</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>3.3603</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>4.5732</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>2.9913</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>2.3382</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>out!$F$10:$F$14</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>4.8032</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0.8694</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>6.1606</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>out!$D$4:$D$8</c:f>
@@ -517,10 +343,11 @@
             <c:v>4 PS</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="41275" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -529,84 +356,13 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>out!$G$16:$G$20</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>1.2781</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.1508</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>6.7194</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3.5249</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>1.1707</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>out!$F$16:$F$20</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.9627</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.0133</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.0584</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>26.9899</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>13.0162</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>out!$D$4:$D$8</c:f>
@@ -664,10 +420,11 @@
             <c:v>8 PS</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="53975" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -676,84 +433,13 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>out!$G$22:$G$26</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.4353</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.6815</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.155</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>41.4111</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>4.1937</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>out!$F$22:$F$26</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.2113</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.9761</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.0283</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>9.3025</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>20.7719</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>out!$D$4:$D$8</c:f>
@@ -812,13 +498,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2106070800"/>
-        <c:axId val="-2108586480"/>
+        <c:axId val="-2118892720"/>
+        <c:axId val="-2118886496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2106070800"/>
+        <c:axId val="-2118892720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="32.0"/>
+          <c:min val="2.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -843,7 +531,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -856,7 +544,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1100">
+                  <a:rPr lang="en-US" sz="1600" b="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -880,7 +568,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -902,12 +590,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="47625" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -918,7 +603,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -933,14 +618,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2108586480"/>
+        <c:crossAx val="-2118886496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2108586480"/>
+        <c:axId val="-2118886496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="45.0"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -965,7 +652,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -978,30 +665,24 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1100">
+                  <a:rPr lang="en-US" sz="1600" b="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Percentage</a:t>
+                  <a:t>Percentage Improvement</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t> Improvement: Agg+No Multicast over Baseline</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="1100">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.00560747663551402"/>
+              <c:y val="0.245325197869024"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1015,7 +696,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1037,23 +718,20 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="47625" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1068,7 +746,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2106070800"/>
+        <c:crossAx val="-2118892720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1086,9 +764,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.101422474059901"/>
-          <c:y val="0.182729319249065"/>
-          <c:w val="0.481857384649349"/>
+          <c:x val="0.08086172639635"/>
+          <c:y val="0.0662998237768791"/>
+          <c:w val="0.879988225770844"/>
           <c:h val="0.0488360106345051"/>
         </c:manualLayout>
       </c:layout>
@@ -1105,7 +783,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -1169,82 +847,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Inception-V3: Percentage</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t> Improvement vs. Number of Workers (Multicast/No Aggregation vs Baseline)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1600" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.102257217847769"/>
+          <c:y val="0.0381523530488921"/>
+          <c:w val="0.867097057893941"/>
+          <c:h val="0.836362082646646"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -1255,7 +870,7 @@
             <c:v>1 PS</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -1267,84 +882,13 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>out!$G$29:$G$33</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.4963</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.1687</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.6782</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3.3384</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>1.3854</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>out!$F$29:$F$33</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>1.0506</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>2.4275</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.5733</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1.8999</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>1.2617</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>out!$D$4:$D$8</c:f>
@@ -1402,10 +946,11 @@
             <c:v>2 PS</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="C00000"/>
               </a:solidFill>
+              <a:prstDash val="lgDashDotDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1414,84 +959,13 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>out!$G$35:$G$39</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.0238</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.2197</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.933</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0.8437</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>1.1974</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>out!$F$35:$F$39</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.0486</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>3.0315</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.6651</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1.5857</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0.7211</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>out!$D$4:$D$8</c:f>
@@ -1549,10 +1023,11 @@
             <c:v>4 PS</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1561,84 +1036,13 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>out!$G$41:$G$45</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.7904</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.5128</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.8812</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>8.535</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0.8289</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>out!$F$41:$F$45</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.5842</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>1.428</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.9092</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>2.2585</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0.8131</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>out!$D$4:$D$8</c:f>
@@ -1696,10 +1100,11 @@
             <c:v>8 PS</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="47625" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1708,84 +1113,13 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>out!$G$47:$G$51</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.5778</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.8622</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.7364</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>34.3139</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0.842</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>out!$F$47:$F$51</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.0319</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.5418</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.682</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>19.5926</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>9.5029</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>out!$D$4:$D$8</c:f>
@@ -1844,13 +1178,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2103936240"/>
-        <c:axId val="-2103929984"/>
+        <c:axId val="-2118845520"/>
+        <c:axId val="-2118839296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2103936240"/>
+        <c:axId val="-2118845520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="32.0"/>
+          <c:min val="2.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1875,7 +1211,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1888,7 +1224,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1100">
+                  <a:rPr lang="en-US" sz="1600">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -1912,7 +1248,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1934,12 +1270,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="47625" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1950,7 +1283,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1965,14 +1298,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2103929984"/>
+        <c:crossAx val="-2118839296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2103929984"/>
+        <c:axId val="-2118839296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="60.0"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2010,26 +1345,13 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1100">
+                  <a:rPr lang="en-US" sz="1600">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Percentage</a:t>
+                  <a:t>Percentage Improvement</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t> Improvement: Multicast+No Agg over Baseline</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="1100">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2069,12 +1391,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="47625" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -2085,7 +1404,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2100,13 +1419,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2103936240"/>
+        <c:crossAx val="-2118845520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="10.0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="25400">
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
@@ -2118,9 +1438,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0920662705265931"/>
-          <c:y val="0.167205386519441"/>
-          <c:w val="0.499569270848579"/>
+          <c:x val="0.10321868688347"/>
+          <c:y val="0.0559505352904626"/>
+          <c:w val="0.843373871459785"/>
           <c:h val="0.0488360106345051"/>
         </c:manualLayout>
       </c:layout>
@@ -2137,7 +1457,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -2201,82 +1521,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Inception-V3: Percentage</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t> Improvement vs. Number of Workers (Aggregation/Multicast vs Baseline)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1600" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10749281994201"/>
+          <c:y val="0.0380540222420651"/>
+          <c:w val="0.855665993321515"/>
+          <c:h val="0.846687636983521"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -2287,7 +1544,7 @@
             <c:v>1 PS</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -2299,84 +1556,13 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>out!$G$54:$G$58</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.4963</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>3.4201</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>4.3108</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1.5144</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0.9357</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>out!$F$54:$F$58</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>1.0506</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>2.4597</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>4.6616</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>6.5517</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>3.7612</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>out!$D$4:$D$8</c:f>
@@ -2434,10 +1620,11 @@
             <c:v>2 PS</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="C00000"/>
               </a:solidFill>
+              <a:prstDash val="lgDashDotDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2446,84 +1633,13 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>out!$G$60:$G$64</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.0238</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>3.5396</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>3.8494</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0.1876</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0.1219</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>out!$F$60:$F$64</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.0486</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>3.0719</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>4.1776</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0.4435</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>13.6037</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>out!$D$4:$D$8</c:f>
@@ -2581,10 +1697,11 @@
             <c:v>4 PS</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2593,84 +1710,13 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>out!$G$66:$G$70</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.7904</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.5128</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>6.2503</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>5.9524</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0.654</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>out!$F$66:$F$70</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.5842</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>1.428</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>1.4247</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>26.1351</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>8.83</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>out!$D$4:$D$8</c:f>
@@ -2728,10 +1774,11 @@
             <c:v>8 PS</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="47625" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2740,84 +1787,13 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>out!$G$72:$G$76</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.5778</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.8622</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.7364</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>30.5061</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0.4658</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>out!$F$72:$F$76</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.0319</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.5418</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.682</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>12.2631</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>4.2102</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>out!$D$4:$D$8</c:f>
@@ -2876,13 +1852,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2103871344"/>
-        <c:axId val="-2103865088"/>
+        <c:axId val="-2118871728"/>
+        <c:axId val="-2118865504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2103871344"/>
+        <c:axId val="-2118871728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="32.0"/>
+          <c:min val="2.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2907,7 +1885,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2920,7 +1898,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1100">
+                  <a:rPr lang="en-US" sz="1600">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -2944,7 +1922,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -2966,12 +1944,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="47625" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -2982,7 +1957,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2997,14 +1972,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2103865088"/>
+        <c:crossAx val="-2118865504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2103865088"/>
+        <c:axId val="-2118865504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100.0"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3042,7 +2019,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1100">
+                  <a:rPr lang="en-US" sz="1600">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -3050,18 +2027,13 @@
                   <a:t>Percentage</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1100" baseline="0">
+                  <a:rPr lang="en-US" sz="1600" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t> Improvement: Multicast+Agg over Baseline</a:t>
+                  <a:t> Improvement</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="1100">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3101,12 +2073,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="47625" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -3117,7 +2086,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3132,7 +2101,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2103871344"/>
+        <c:crossAx val="-2118871728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3150,9 +2119,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0902075661594932"/>
-          <c:y val="0.203427896221899"/>
-          <c:w val="0.494903430509264"/>
+          <c:x val="0.133837517692487"/>
+          <c:y val="0.056520618556701"/>
+          <c:w val="0.800313586456143"/>
           <c:h val="0.0488360106345051"/>
         </c:manualLayout>
       </c:layout>
@@ -3169,7 +2138,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -3233,82 +2202,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Inception-V3: Percentage</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t> Improvement vs. Number of Workers (Multicast+Agg vs Multicast)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1600" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.104710530293661"/>
+          <c:y val="0.0336351875808538"/>
+          <c:w val="0.864643745448049"/>
+          <c:h val="0.82993063124548"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -3319,7 +2225,7 @@
             <c:v>1 PS</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -3331,84 +2237,13 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>out!$G$79:$G$83</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.0202</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>4.1939</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>6.9352</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0.6827</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>1.94</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>out!$F$79:$F$83</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>7.465</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>8.9237</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>6.4278</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>out!$D$4:$D$8</c:f>
@@ -3466,10 +2301,11 @@
             <c:v>2 PS</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="C00000"/>
               </a:solidFill>
+              <a:prstDash val="lgDashDotDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -3478,84 +2314,13 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>out!$G$85:$G$89</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>4.5637</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>7.3087</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1.5184</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0.4937</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>out!$F$85:$F$89</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>7.9035</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0.6049</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>28.0233</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>out!$D$4:$D$8</c:f>
@@ -3613,10 +2378,11 @@
             <c:v>4 PS</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -3625,84 +2391,13 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>out!$G$91:$G$95</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>9.2181</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>6.1464</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0.9307</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>out!$F$91:$F$95</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>38.0281</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>15.0583</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>out!$D$4:$D$8</c:f>
@@ -3760,10 +2455,11 @@
             <c:v>8 PS</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="47625" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -3772,84 +2468,13 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>out!$G$97:$G$101</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>15.1643</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>8.8231</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>out!$F$97:$F$101</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.0</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>21.3811</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>3.7778</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>out!$D$4:$D$8</c:f>
@@ -3908,13 +2533,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2103806640"/>
-        <c:axId val="-2103800384"/>
+        <c:axId val="-2087567040"/>
+        <c:axId val="-2087560816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2103806640"/>
+        <c:axId val="-2087567040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="32.0"/>
+          <c:min val="2.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -3939,7 +2566,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -3952,7 +2579,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1100">
+                  <a:rPr lang="en-US" sz="1600">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -3976,7 +2603,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -3998,12 +2625,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="47625" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -4014,7 +2638,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4029,14 +2653,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2103800384"/>
+        <c:crossAx val="-2087560816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2103800384"/>
+        <c:axId val="-2087560816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4061,7 +2686,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -4074,26 +2699,13 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1100">
+                  <a:rPr lang="en-US" sz="1600">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Percentage</a:t>
+                  <a:t>Percentage Improvement</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t> Improvement: Multicast+Agg over Multicast</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="1100">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -4111,7 +2723,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -4133,12 +2745,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="47625" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -4149,7 +2758,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4164,7 +2773,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2103806640"/>
+        <c:crossAx val="-2087567040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4182,9 +2791,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0902076008949066"/>
-          <c:y val="0.174967352884253"/>
-          <c:w val="0.49458973762966"/>
+          <c:x val="0.123366450921384"/>
+          <c:y val="0.0611251795336708"/>
+          <c:w val="0.824432672355746"/>
           <c:h val="0.0488360106345051"/>
         </c:manualLayout>
       </c:layout>
@@ -4201,7 +2810,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -6480,15 +5089,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6510,15 +5119,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6542,15 +5151,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6574,15 +5183,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>101</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6869,15 +5478,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="Q98" sqref="Q98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6899,8 +5508,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -6914,7 +5526,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -6922,7 +5534,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
@@ -6945,7 +5557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0</v>
       </c>
@@ -6968,7 +5580,7 @@
         <v>3.2835999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0</v>
       </c>
@@ -6991,7 +5603,7 @@
         <v>3.7940999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0</v>
       </c>
@@ -7014,7 +5626,7 @@
         <v>3.8944999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0</v>
       </c>
@@ -7037,7 +5649,7 @@
         <v>1.9033</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0</v>
       </c>
@@ -7060,7 +5672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0</v>
       </c>
@@ -7083,7 +5695,7 @@
         <v>3.3603000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0</v>
       </c>
@@ -7106,7 +5718,7 @@
         <v>4.5731999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0</v>
       </c>
@@ -7129,7 +5741,7 @@
         <v>2.9912999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0</v>
       </c>
@@ -7152,7 +5764,7 @@
         <v>2.3382000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0</v>
       </c>
@@ -7175,7 +5787,7 @@
         <v>1.2781</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0</v>
       </c>
@@ -7198,7 +5810,7 @@
         <v>0.15079999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0</v>
       </c>
@@ -7221,7 +5833,7 @@
         <v>6.7194000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0</v>
       </c>
@@ -7244,7 +5856,7 @@
         <v>3.5249000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>0</v>
       </c>
@@ -7267,7 +5879,7 @@
         <v>1.1707000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>0</v>
       </c>
@@ -7290,7 +5902,7 @@
         <v>0.43530000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>0</v>
       </c>
@@ -7313,7 +5925,7 @@
         <v>0.68149999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>0</v>
       </c>
@@ -7336,7 +5948,7 @@
         <v>0.155</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>0</v>
       </c>
@@ -7359,7 +5971,7 @@
         <v>41.411099999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>0</v>
       </c>
@@ -7382,15 +5994,18 @@
         <v>4.1936999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>12</v>
       </c>
       <c r="B28" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K28" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -7413,7 +6028,7 @@
         <v>0.49630000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -7436,7 +6051,7 @@
         <v>0.16869999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -7459,7 +6074,7 @@
         <v>0.67820000000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -7781,7 +6396,7 @@
         <v>0.86219999999999997</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1</v>
       </c>
@@ -7804,7 +6419,7 @@
         <v>0.73640000000000005</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1</v>
       </c>
@@ -7827,7 +6442,7 @@
         <v>34.313899999999997</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1</v>
       </c>
@@ -7850,7 +6465,7 @@
         <v>0.84199999999999997</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -7858,7 +6473,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1</v>
       </c>
@@ -7881,7 +6496,7 @@
         <v>0.49630000000000002</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1</v>
       </c>
@@ -7903,8 +6518,11 @@
       <c r="G55">
         <v>3.4201000000000001</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K55" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1</v>
       </c>
@@ -7927,7 +6545,7 @@
         <v>4.3108000000000004</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1</v>
       </c>
@@ -7950,7 +6568,7 @@
         <v>1.5144</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1</v>
       </c>
@@ -7973,7 +6591,7 @@
         <v>0.93569999999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1</v>
       </c>
@@ -7996,7 +6614,7 @@
         <v>2.3800000000000002E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1</v>
       </c>
@@ -8019,7 +6637,7 @@
         <v>3.5396000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1</v>
       </c>
@@ -8042,7 +6660,7 @@
         <v>3.8494000000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1</v>
       </c>
@@ -8065,7 +6683,7 @@
         <v>0.18759999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>1</v>
       </c>
@@ -8369,7 +6987,7 @@
         <v>4.1939000000000002</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>1</v>
       </c>
@@ -8392,7 +7010,7 @@
         <v>6.9352</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1</v>
       </c>
@@ -8414,8 +7032,11 @@
       <c r="G82">
         <v>0.68269999999999997</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="L82" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>1</v>
       </c>
@@ -8438,7 +7059,7 @@
         <v>1.94</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>1</v>
       </c>
@@ -8461,7 +7082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>1</v>
       </c>
@@ -8484,7 +7105,7 @@
         <v>4.5636999999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>1</v>
       </c>
@@ -8507,7 +7128,7 @@
         <v>7.3087</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>1</v>
       </c>
@@ -8530,7 +7151,7 @@
         <v>1.5184</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>1</v>
       </c>
@@ -8553,7 +7174,7 @@
         <v>0.49370000000000003</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>1</v>
       </c>
@@ -8576,7 +7197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>1</v>
       </c>
@@ -8599,7 +7220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>1</v>
       </c>
@@ -8622,7 +7243,7 @@
         <v>9.2180999999999997</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>1</v>
       </c>
@@ -8645,7 +7266,7 @@
         <v>6.1463999999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>1</v>
       </c>

</xml_diff>